<commit_message>
Act of completion and TovarChek docs as module
</commit_message>
<xml_diff>
--- a/app/templates/act_tpl.xlsx
+++ b/app/templates/act_tpl.xlsx
@@ -87,7 +87,7 @@
     <t>{{ garanty }}</t>
   </si>
   <si>
-    <t>Всего оказано услуг на сумму: {{ total_as_text.decode("utf-8") }} рублей 00 копеек</t>
+    <t>Всего оказано услуг на сумму: {{ total_as_text.decode("utf-8") }}</t>
   </si>
 </sst>
 </file>
@@ -698,11 +698,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="3.33203125" customWidth="1"/>
-    <col min="5" max="24" width="3.5" customWidth="1"/>
-    <col min="25" max="25" width="5.33203125" customWidth="1"/>
-    <col min="26" max="26" width="6.83203125" customWidth="1"/>
-    <col min="27" max="256" width="3.5" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="4" width="3.1640625" customWidth="1"/>
+    <col min="5" max="5" width="3.33203125" customWidth="1"/>
+    <col min="6" max="20" width="3.5" customWidth="1"/>
+    <col min="21" max="21" width="4.1640625" customWidth="1"/>
+    <col min="22" max="22" width="3.83203125" customWidth="1"/>
+    <col min="23" max="23" width="3.5" customWidth="1"/>
+    <col min="24" max="24" width="4.5" customWidth="1"/>
+    <col min="25" max="25" width="4.1640625" customWidth="1"/>
+    <col min="26" max="26" width="4.6640625" customWidth="1"/>
+    <col min="27" max="27" width="3.5" customWidth="1"/>
+    <col min="28" max="28" width="3" customWidth="1"/>
+    <col min="29" max="29" width="3.33203125" customWidth="1"/>
+    <col min="30" max="31" width="3.1640625" customWidth="1"/>
+    <col min="32" max="32" width="3.33203125" customWidth="1"/>
+    <col min="33" max="33" width="3.1640625" customWidth="1"/>
+    <col min="34" max="256" width="3.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:34" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>